<commit_message>
finished input list generation and sanity checks.
</commit_message>
<xml_diff>
--- a/scene_cat_exp_2023.2/input_files/10_scenecat_block_order.xlsx
+++ b/scene_cat_exp_2023.2/input_files/10_scenecat_block_order.xlsx
@@ -360,32 +360,32 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>bedrooms_1</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
           <t>kitchens_1</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>living_rooms_1</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>bedrooms_2</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>kitchens_2</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>living_rooms_2</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>bedrooms_1</t>
+        </is>
+      </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>living_rooms_2</t>
+          <t>bedrooms_2</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
elaborated sanity checks. increased the proportion of new images in memory task.
</commit_message>
<xml_diff>
--- a/scene_cat_exp_2023.2/input_files/10_scenecat_block_order.xlsx
+++ b/scene_cat_exp_2023.2/input_files/10_scenecat_block_order.xlsx
@@ -360,32 +360,32 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>kitchens_1</t>
+          <t>bedrooms_1</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>bedrooms_2</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>living_rooms_1</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>kitchens_1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>kitchens_2</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>living_rooms_2</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>bedrooms_1</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>bedrooms_2</t>
         </is>
       </c>
     </row>

</xml_diff>